<commit_message>
Revert "Update week 6 du.xlsx"
This reverts commit 5f680fc98e365a930440fda304e1678053bbddd7.
</commit_message>
<xml_diff>
--- a/metrics/week 6 du.xlsx
+++ b/metrics/week 6 du.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gordon\SMU\IS212\GitHub\project-g3t4\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E060569-4446-4BBD-98B9-D8EDE5C1B91C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5F54739-0683-44AE-872F-860D0D83DA5D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="38">
   <si>
     <t>Person</t>
   </si>
@@ -99,6 +99,9 @@
     <t>Start coding DAOs</t>
   </si>
   <si>
+    <t>NIL</t>
+  </si>
+  <si>
     <t>Start coding common files (eg. connection manager, protect)</t>
   </si>
   <si>
@@ -142,30 +145,6 @@
   </si>
   <si>
     <t>Realised there were many things to think about on scheduling</t>
-  </si>
-  <si>
-    <t>Code BiddingRoundDAO, Round1DAO, admin home</t>
-  </si>
-  <si>
-    <t>Code admin controls, eg. navigation for bootstrap, round management</t>
-  </si>
-  <si>
-    <t>Difficulty coding Round 1 related DAOs without Round 1 clearing logic code</t>
-  </si>
-  <si>
-    <t>Replace session authentication with token authentication for student</t>
-  </si>
-  <si>
-    <t>Replace session authentication with token authentication for admin</t>
-  </si>
-  <si>
-    <t>Initially, wasn't sure that we were supposed to pass token using $_GET on every page</t>
-  </si>
-  <si>
-    <t>Code boostrap</t>
-  </si>
-  <si>
-    <t>No issues</t>
   </si>
 </sst>
 </file>
@@ -540,7 +519,7 @@
   </sheetPr>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="E16" sqref="E16"/>
     </sheetView>
@@ -643,14 +622,12 @@
         <v>18</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
-      <c r="F3" s="7" t="s">
-        <v>40</v>
-      </c>
+      <c r="F3" s="7"/>
       <c r="G3" s="7"/>
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
@@ -661,17 +638,15 @@
         <v>11</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
-      <c r="F4" s="7" t="s">
-        <v>41</v>
-      </c>
+      <c r="F4" s="7"/>
       <c r="G4" s="7"/>
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
@@ -682,17 +657,15 @@
         <v>12</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
-      <c r="F5" s="7" t="s">
-        <v>42</v>
-      </c>
+      <c r="F5" s="7"/>
       <c r="G5" s="7"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -708,14 +681,12 @@
         <v>18</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
-      <c r="F6" s="7" t="s">
-        <v>40</v>
-      </c>
+      <c r="F6" s="7"/>
       <c r="G6" s="7"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -726,17 +697,15 @@
         <v>14</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
-      <c r="F7" s="7" t="s">
-        <v>41</v>
-      </c>
+      <c r="F7" s="7"/>
       <c r="G7" s="7"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -747,17 +716,15 @@
         <v>12</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
-      <c r="F8" s="7" t="s">
-        <v>42</v>
-      </c>
+      <c r="F8" s="7"/>
       <c r="G8" s="7"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -773,14 +740,12 @@
         <v>18</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
-      <c r="F9" s="7" t="s">
-        <v>37</v>
-      </c>
+      <c r="F9" s="7"/>
       <c r="G9" s="7"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -794,14 +759,12 @@
         <v>21</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
-      <c r="F10" s="7" t="s">
-        <v>38</v>
-      </c>
+      <c r="F10" s="7"/>
       <c r="G10" s="7"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -812,17 +775,15 @@
         <v>12</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
-      <c r="F11" s="7" t="s">
-        <v>39</v>
-      </c>
+      <c r="F11" s="7"/>
       <c r="G11" s="7"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
@@ -838,14 +799,12 @@
         <v>18</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
-      <c r="F12" s="7" t="s">
-        <v>37</v>
-      </c>
+      <c r="F12" s="7"/>
       <c r="G12" s="7"/>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
@@ -859,14 +818,12 @@
         <v>21</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
-      <c r="F13" s="7" t="s">
-        <v>38</v>
-      </c>
+      <c r="F13" s="7"/>
       <c r="G13" s="7"/>
       <c r="H13" s="6"/>
       <c r="I13" s="6"/>
@@ -877,17 +834,15 @@
         <v>12</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
-      <c r="F14" s="7" t="s">
-        <v>39</v>
-      </c>
+      <c r="F14" s="7"/>
       <c r="G14" s="7"/>
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
@@ -906,11 +861,9 @@
         <v>18</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
-      <c r="F15" s="7" t="s">
-        <v>18</v>
-      </c>
+      <c r="F15" s="7"/>
       <c r="G15" s="7"/>
       <c r="H15" s="6"/>
       <c r="I15" s="6"/>
@@ -924,14 +877,12 @@
         <v>18</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E16" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="F16" s="7" t="s">
-        <v>43</v>
-      </c>
+      <c r="F16" s="7"/>
       <c r="G16" s="7"/>
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
@@ -942,17 +893,15 @@
         <v>12</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
-      <c r="F17" s="7" t="s">
-        <v>44</v>
-      </c>
+      <c r="F17" s="7"/>
       <c r="G17" s="7"/>
       <c r="H17" s="6"/>
       <c r="I17" s="6"/>

</xml_diff>